<commit_message>
Added the new master file and template adjustment.
</commit_message>
<xml_diff>
--- a/storage/system/master.xlsx
+++ b/storage/system/master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\payhp\storage\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBCE9DC-3B1F-4E0F-917A-4D6A628DA287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9435E8-1EA1-4BC8-8A7C-5405401662CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
   <si>
     <t>STATUS</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>ADDITIONAL PAY</t>
-  </si>
-  <si>
-    <t>PAYMENTS</t>
   </si>
   <si>
     <t>ENABLE</t>
@@ -198,12 +195,66 @@
   <si>
     <t>mariaquizumbing@ahmoutsourcing.com</t>
   </si>
+  <si>
+    <t>CONTRIBUTIONS</t>
+  </si>
+  <si>
+    <t>LOANS</t>
+  </si>
+  <si>
+    <t>HDMF</t>
+  </si>
+  <si>
+    <t>E25</t>
+  </si>
+  <si>
+    <t>E26</t>
+  </si>
+  <si>
+    <t>E27</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>EMAIL ADDRESS</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>AMT</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>TERM</t>
+  </si>
+  <si>
+    <t>1,12</t>
+  </si>
+  <si>
+    <t>4,12</t>
+  </si>
+  <si>
+    <t>8,12</t>
+  </si>
+  <si>
+    <t>LEAVE CREDIT</t>
+  </si>
+  <si>
+    <t>DAY.HRS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,8 +389,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +592,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,12 +814,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -764,16 +825,20 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1131,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y200"/>
+  <dimension ref="A1:AD200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,308 +1221,365 @@
     <col min="16" max="17" width="9.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.28515625" customWidth="1"/>
     <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="30" max="30" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="5" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="5" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="6"/>
-    </row>
-    <row r="2" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1234567890</v>
-      </c>
-      <c r="I4" s="1">
-        <v>20600</v>
-      </c>
-      <c r="J4" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K4" s="1">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1">
-        <v>500</v>
-      </c>
-      <c r="M4" s="1">
-        <v>70</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>425</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1">
-        <v>30</v>
-      </c>
-      <c r="X4" s="1">
-        <v>525</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H5" s="1">
         <v>1234567890</v>
       </c>
       <c r="I5" s="1">
-        <v>30500</v>
+        <v>20600</v>
       </c>
       <c r="J5" s="1">
-        <v>7000</v>
+        <v>3000</v>
       </c>
       <c r="K5" s="1">
         <v>26</v>
@@ -1502,39 +1624,48 @@
         <v>525</v>
       </c>
       <c r="Y5" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>120</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H6" s="1">
         <v>1234567890</v>
       </c>
       <c r="I6" s="1">
-        <v>15060</v>
+        <v>30500</v>
       </c>
       <c r="J6" s="1">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="K6" s="1">
         <v>26</v>
@@ -1579,37 +1710,113 @@
         <v>525</v>
       </c>
       <c r="Y6" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1">
+        <v>450</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="I7" s="1">
+        <v>15060</v>
+      </c>
+      <c r="J7" s="1">
+        <v>500</v>
+      </c>
+      <c r="K7" s="1">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1">
+        <v>500</v>
+      </c>
+      <c r="M7" s="1">
+        <v>70</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>425</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>30</v>
+      </c>
+      <c r="X7" s="1">
+        <v>525</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>360</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>230</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1635,8 +1842,13 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1662,8 +1874,13 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1689,8 +1906,13 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1716,8 +1938,13 @@
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1743,8 +1970,13 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1770,8 +2002,13 @@
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1797,8 +2034,13 @@
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1824,8 +2066,13 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1851,8 +2098,13 @@
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1878,8 +2130,13 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1905,8 +2162,13 @@
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1932,8 +2194,13 @@
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1959,8 +2226,13 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1986,8 +2258,13 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2013,8 +2290,13 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2040,8 +2322,13 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2067,8 +2354,13 @@
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2094,8 +2386,13 @@
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2121,8 +2418,13 @@
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2148,8 +2450,13 @@
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2175,8 +2482,13 @@
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2202,8 +2514,13 @@
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2229,8 +2546,13 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2256,8 +2578,13 @@
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="6"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2283,8 +2610,13 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2310,8 +2642,13 @@
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="6"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2337,8 +2674,13 @@
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="6"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2364,8 +2706,13 @@
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2391,8 +2738,13 @@
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="6"/>
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="6"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2418,8 +2770,13 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6"/>
+      <c r="AC37" s="6"/>
+      <c r="AD37" s="6"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2445,8 +2802,13 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="6"/>
+      <c r="AB38" s="6"/>
+      <c r="AC38" s="6"/>
+      <c r="AD38" s="6"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2472,8 +2834,13 @@
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6"/>
+      <c r="AC39" s="6"/>
+      <c r="AD39" s="6"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2499,8 +2866,13 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="6"/>
+      <c r="AB40" s="6"/>
+      <c r="AC40" s="6"/>
+      <c r="AD40" s="6"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2526,8 +2898,13 @@
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="6"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2553,8 +2930,13 @@
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="6"/>
+      <c r="AB42" s="6"/>
+      <c r="AC42" s="6"/>
+      <c r="AD42" s="6"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2580,8 +2962,13 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="6"/>
+      <c r="AB43" s="6"/>
+      <c r="AC43" s="6"/>
+      <c r="AD43" s="6"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2607,8 +2994,13 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="6"/>
+      <c r="AB44" s="6"/>
+      <c r="AC44" s="6"/>
+      <c r="AD44" s="6"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2634,8 +3026,13 @@
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="6"/>
+      <c r="AB45" s="6"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="6"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2661,8 +3058,13 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6"/>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2688,8 +3090,13 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6"/>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2715,8 +3122,13 @@
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6"/>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2742,8 +3154,13 @@
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="6"/>
+      <c r="AB49" s="6"/>
+      <c r="AC49" s="6"/>
+      <c r="AD49" s="6"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2769,8 +3186,13 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="6"/>
+      <c r="AB50" s="6"/>
+      <c r="AC50" s="6"/>
+      <c r="AD50" s="6"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2796,8 +3218,13 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
       <c r="Y51" s="1"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2823,8 +3250,13 @@
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
       <c r="Y52" s="1"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="6"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="6"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2850,8 +3282,13 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
       <c r="Y53" s="1"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="6"/>
+      <c r="AB53" s="6"/>
+      <c r="AC53" s="6"/>
+      <c r="AD53" s="6"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2877,8 +3314,13 @@
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
       <c r="Y54" s="1"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="6"/>
+      <c r="AB54" s="6"/>
+      <c r="AC54" s="6"/>
+      <c r="AD54" s="6"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2904,8 +3346,13 @@
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
       <c r="Y55" s="1"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="6"/>
+      <c r="AB55" s="6"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55" s="6"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2931,8 +3378,13 @@
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
       <c r="Y56" s="1"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="6"/>
+      <c r="AB56" s="6"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="6"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2958,8 +3410,13 @@
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
       <c r="Y57" s="1"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="6"/>
+      <c r="AB57" s="6"/>
+      <c r="AC57" s="6"/>
+      <c r="AD57" s="6"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2985,8 +3442,13 @@
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
       <c r="Y58" s="1"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="6"/>
+      <c r="AB58" s="6"/>
+      <c r="AC58" s="6"/>
+      <c r="AD58" s="6"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3012,8 +3474,13 @@
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
       <c r="Y59" s="1"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="6"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3039,8 +3506,13 @@
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
       <c r="Y60" s="1"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="6"/>
+      <c r="AB60" s="6"/>
+      <c r="AC60" s="6"/>
+      <c r="AD60" s="6"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3066,8 +3538,13 @@
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
       <c r="Y61" s="1"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="6"/>
+      <c r="AB61" s="6"/>
+      <c r="AC61" s="6"/>
+      <c r="AD61" s="6"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3093,8 +3570,13 @@
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
       <c r="Y62" s="1"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="6"/>
+      <c r="AB62" s="6"/>
+      <c r="AC62" s="6"/>
+      <c r="AD62" s="6"/>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3120,8 +3602,13 @@
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
       <c r="Y63" s="1"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="6"/>
+      <c r="AB63" s="6"/>
+      <c r="AC63" s="6"/>
+      <c r="AD63" s="6"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3147,8 +3634,13 @@
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
       <c r="Y64" s="1"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="6"/>
+      <c r="AB64" s="6"/>
+      <c r="AC64" s="6"/>
+      <c r="AD64" s="6"/>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3174,8 +3666,13 @@
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
       <c r="Y65" s="1"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="6"/>
+      <c r="AC65" s="6"/>
+      <c r="AD65" s="6"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3201,8 +3698,13 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
       <c r="Y66" s="1"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="6"/>
+      <c r="AB66" s="6"/>
+      <c r="AC66" s="6"/>
+      <c r="AD66" s="6"/>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3228,8 +3730,13 @@
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
       <c r="Y67" s="1"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="6"/>
+      <c r="AB67" s="6"/>
+      <c r="AC67" s="6"/>
+      <c r="AD67" s="6"/>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -3255,8 +3762,13 @@
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="6"/>
+      <c r="AB68" s="6"/>
+      <c r="AC68" s="6"/>
+      <c r="AD68" s="6"/>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3282,8 +3794,13 @@
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="6"/>
+      <c r="AB69" s="6"/>
+      <c r="AC69" s="6"/>
+      <c r="AD69" s="6"/>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3309,8 +3826,13 @@
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="6"/>
+      <c r="AB70" s="6"/>
+      <c r="AC70" s="6"/>
+      <c r="AD70" s="6"/>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3336,8 +3858,13 @@
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="6"/>
+      <c r="AB71" s="6"/>
+      <c r="AC71" s="6"/>
+      <c r="AD71" s="6"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -3363,8 +3890,13 @@
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="6"/>
+      <c r="AB72" s="6"/>
+      <c r="AC72" s="6"/>
+      <c r="AD72" s="6"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3390,8 +3922,13 @@
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
       <c r="Y73" s="1"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="6"/>
+      <c r="AB73" s="6"/>
+      <c r="AC73" s="6"/>
+      <c r="AD73" s="6"/>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3417,8 +3954,13 @@
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
       <c r="Y74" s="1"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+      <c r="AC74" s="6"/>
+      <c r="AD74" s="6"/>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -3444,8 +3986,13 @@
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
       <c r="Y75" s="1"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+      <c r="AC75" s="6"/>
+      <c r="AD75" s="6"/>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -3471,8 +4018,13 @@
       <c r="W76" s="1"/>
       <c r="X76" s="1"/>
       <c r="Y76" s="1"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="6"/>
+      <c r="AB76" s="6"/>
+      <c r="AC76" s="6"/>
+      <c r="AD76" s="6"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3498,8 +4050,13 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
       <c r="Y77" s="1"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3525,8 +4082,13 @@
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
       <c r="Y78" s="1"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z78" s="1"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -3552,8 +4114,13 @@
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
       <c r="Y79" s="1"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z79" s="1"/>
+      <c r="AA79" s="6"/>
+      <c r="AB79" s="6"/>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -3579,8 +4146,13 @@
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
       <c r="Y80" s="1"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z80" s="1"/>
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+      <c r="AC80" s="6"/>
+      <c r="AD80" s="6"/>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -3606,8 +4178,13 @@
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
       <c r="Y81" s="1"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z81" s="1"/>
+      <c r="AA81" s="6"/>
+      <c r="AB81" s="6"/>
+      <c r="AC81" s="6"/>
+      <c r="AD81" s="6"/>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -3633,8 +4210,13 @@
       <c r="W82" s="1"/>
       <c r="X82" s="1"/>
       <c r="Y82" s="1"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z82" s="1"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -3660,8 +4242,13 @@
       <c r="W83" s="1"/>
       <c r="X83" s="1"/>
       <c r="Y83" s="1"/>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z83" s="1"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -3687,8 +4274,13 @@
       <c r="W84" s="1"/>
       <c r="X84" s="1"/>
       <c r="Y84" s="1"/>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z84" s="1"/>
+      <c r="AA84" s="6"/>
+      <c r="AB84" s="6"/>
+      <c r="AC84" s="6"/>
+      <c r="AD84" s="6"/>
+    </row>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3714,8 +4306,13 @@
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
       <c r="Y85" s="1"/>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z85" s="1"/>
+      <c r="AA85" s="6"/>
+      <c r="AB85" s="6"/>
+      <c r="AC85" s="6"/>
+      <c r="AD85" s="6"/>
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -3741,8 +4338,13 @@
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
       <c r="Y86" s="1"/>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z86" s="1"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
+      <c r="AC86" s="6"/>
+      <c r="AD86" s="6"/>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3768,8 +4370,13 @@
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
       <c r="Y87" s="1"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z87" s="1"/>
+      <c r="AA87" s="6"/>
+      <c r="AB87" s="6"/>
+      <c r="AC87" s="6"/>
+      <c r="AD87" s="6"/>
+    </row>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3795,8 +4402,13 @@
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
       <c r="Y88" s="1"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z88" s="1"/>
+      <c r="AA88" s="6"/>
+      <c r="AB88" s="6"/>
+      <c r="AC88" s="6"/>
+      <c r="AD88" s="6"/>
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3822,8 +4434,13 @@
       <c r="W89" s="1"/>
       <c r="X89" s="1"/>
       <c r="Y89" s="1"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z89" s="1"/>
+      <c r="AA89" s="6"/>
+      <c r="AB89" s="6"/>
+      <c r="AC89" s="6"/>
+      <c r="AD89" s="6"/>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3849,8 +4466,13 @@
       <c r="W90" s="1"/>
       <c r="X90" s="1"/>
       <c r="Y90" s="1"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z90" s="1"/>
+      <c r="AA90" s="6"/>
+      <c r="AB90" s="6"/>
+      <c r="AC90" s="6"/>
+      <c r="AD90" s="6"/>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3876,8 +4498,13 @@
       <c r="W91" s="1"/>
       <c r="X91" s="1"/>
       <c r="Y91" s="1"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z91" s="1"/>
+      <c r="AA91" s="6"/>
+      <c r="AB91" s="6"/>
+      <c r="AC91" s="6"/>
+      <c r="AD91" s="6"/>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3903,8 +4530,13 @@
       <c r="W92" s="1"/>
       <c r="X92" s="1"/>
       <c r="Y92" s="1"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z92" s="1"/>
+      <c r="AA92" s="6"/>
+      <c r="AB92" s="6"/>
+      <c r="AC92" s="6"/>
+      <c r="AD92" s="6"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3930,8 +4562,13 @@
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
       <c r="Y93" s="1"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z93" s="1"/>
+      <c r="AA93" s="6"/>
+      <c r="AB93" s="6"/>
+      <c r="AC93" s="6"/>
+      <c r="AD93" s="6"/>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3957,8 +4594,13 @@
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
       <c r="Y94" s="1"/>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z94" s="1"/>
+      <c r="AA94" s="6"/>
+      <c r="AB94" s="6"/>
+      <c r="AC94" s="6"/>
+      <c r="AD94" s="6"/>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3984,8 +4626,13 @@
       <c r="W95" s="1"/>
       <c r="X95" s="1"/>
       <c r="Y95" s="1"/>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z95" s="1"/>
+      <c r="AA95" s="6"/>
+      <c r="AB95" s="6"/>
+      <c r="AC95" s="6"/>
+      <c r="AD95" s="6"/>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4011,8 +4658,13 @@
       <c r="W96" s="1"/>
       <c r="X96" s="1"/>
       <c r="Y96" s="1"/>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z96" s="1"/>
+      <c r="AA96" s="6"/>
+      <c r="AB96" s="6"/>
+      <c r="AC96" s="6"/>
+      <c r="AD96" s="6"/>
+    </row>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4038,8 +4690,13 @@
       <c r="W97" s="1"/>
       <c r="X97" s="1"/>
       <c r="Y97" s="1"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z97" s="1"/>
+      <c r="AA97" s="6"/>
+      <c r="AB97" s="6"/>
+      <c r="AC97" s="6"/>
+      <c r="AD97" s="6"/>
+    </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4065,8 +4722,13 @@
       <c r="W98" s="1"/>
       <c r="X98" s="1"/>
       <c r="Y98" s="1"/>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z98" s="1"/>
+      <c r="AA98" s="6"/>
+      <c r="AB98" s="6"/>
+      <c r="AC98" s="6"/>
+      <c r="AD98" s="6"/>
+    </row>
+    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4092,8 +4754,13 @@
       <c r="W99" s="1"/>
       <c r="X99" s="1"/>
       <c r="Y99" s="1"/>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z99" s="1"/>
+      <c r="AA99" s="6"/>
+      <c r="AB99" s="6"/>
+      <c r="AC99" s="6"/>
+      <c r="AD99" s="6"/>
+    </row>
+    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4119,8 +4786,13 @@
       <c r="W100" s="1"/>
       <c r="X100" s="1"/>
       <c r="Y100" s="1"/>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z100" s="1"/>
+      <c r="AA100" s="6"/>
+      <c r="AB100" s="6"/>
+      <c r="AC100" s="6"/>
+      <c r="AD100" s="6"/>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -4146,8 +4818,13 @@
       <c r="W101" s="1"/>
       <c r="X101" s="1"/>
       <c r="Y101" s="1"/>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z101" s="1"/>
+      <c r="AA101" s="6"/>
+      <c r="AB101" s="6"/>
+      <c r="AC101" s="6"/>
+      <c r="AD101" s="6"/>
+    </row>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4173,8 +4850,13 @@
       <c r="W102" s="1"/>
       <c r="X102" s="1"/>
       <c r="Y102" s="1"/>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z102" s="1"/>
+      <c r="AA102" s="6"/>
+      <c r="AB102" s="6"/>
+      <c r="AC102" s="6"/>
+      <c r="AD102" s="6"/>
+    </row>
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4200,8 +4882,13 @@
       <c r="W103" s="1"/>
       <c r="X103" s="1"/>
       <c r="Y103" s="1"/>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z103" s="1"/>
+      <c r="AA103" s="6"/>
+      <c r="AB103" s="6"/>
+      <c r="AC103" s="6"/>
+      <c r="AD103" s="6"/>
+    </row>
+    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4227,8 +4914,13 @@
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
       <c r="Y104" s="1"/>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z104" s="1"/>
+      <c r="AA104" s="6"/>
+      <c r="AB104" s="6"/>
+      <c r="AC104" s="6"/>
+      <c r="AD104" s="6"/>
+    </row>
+    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -4254,8 +4946,13 @@
       <c r="W105" s="1"/>
       <c r="X105" s="1"/>
       <c r="Y105" s="1"/>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="6"/>
+      <c r="AB105" s="6"/>
+      <c r="AC105" s="6"/>
+      <c r="AD105" s="6"/>
+    </row>
+    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -4281,8 +4978,13 @@
       <c r="W106" s="1"/>
       <c r="X106" s="1"/>
       <c r="Y106" s="1"/>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z106" s="1"/>
+      <c r="AA106" s="6"/>
+      <c r="AB106" s="6"/>
+      <c r="AC106" s="6"/>
+      <c r="AD106" s="6"/>
+    </row>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4308,8 +5010,13 @@
       <c r="W107" s="1"/>
       <c r="X107" s="1"/>
       <c r="Y107" s="1"/>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z107" s="1"/>
+      <c r="AA107" s="6"/>
+      <c r="AB107" s="6"/>
+      <c r="AC107" s="6"/>
+      <c r="AD107" s="6"/>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -4335,8 +5042,13 @@
       <c r="W108" s="1"/>
       <c r="X108" s="1"/>
       <c r="Y108" s="1"/>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z108" s="1"/>
+      <c r="AA108" s="6"/>
+      <c r="AB108" s="6"/>
+      <c r="AC108" s="6"/>
+      <c r="AD108" s="6"/>
+    </row>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -4362,8 +5074,13 @@
       <c r="W109" s="1"/>
       <c r="X109" s="1"/>
       <c r="Y109" s="1"/>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z109" s="1"/>
+      <c r="AA109" s="6"/>
+      <c r="AB109" s="6"/>
+      <c r="AC109" s="6"/>
+      <c r="AD109" s="6"/>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -4389,8 +5106,13 @@
       <c r="W110" s="1"/>
       <c r="X110" s="1"/>
       <c r="Y110" s="1"/>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z110" s="1"/>
+      <c r="AA110" s="6"/>
+      <c r="AB110" s="6"/>
+      <c r="AC110" s="6"/>
+      <c r="AD110" s="6"/>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -4416,8 +5138,13 @@
       <c r="W111" s="1"/>
       <c r="X111" s="1"/>
       <c r="Y111" s="1"/>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z111" s="1"/>
+      <c r="AA111" s="6"/>
+      <c r="AB111" s="6"/>
+      <c r="AC111" s="6"/>
+      <c r="AD111" s="6"/>
+    </row>
+    <row r="112" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -4443,8 +5170,13 @@
       <c r="W112" s="1"/>
       <c r="X112" s="1"/>
       <c r="Y112" s="1"/>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z112" s="1"/>
+      <c r="AA112" s="6"/>
+      <c r="AB112" s="6"/>
+      <c r="AC112" s="6"/>
+      <c r="AD112" s="6"/>
+    </row>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -4470,8 +5202,13 @@
       <c r="W113" s="1"/>
       <c r="X113" s="1"/>
       <c r="Y113" s="1"/>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z113" s="1"/>
+      <c r="AA113" s="6"/>
+      <c r="AB113" s="6"/>
+      <c r="AC113" s="6"/>
+      <c r="AD113" s="6"/>
+    </row>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -4497,8 +5234,13 @@
       <c r="W114" s="1"/>
       <c r="X114" s="1"/>
       <c r="Y114" s="1"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z114" s="1"/>
+      <c r="AA114" s="6"/>
+      <c r="AB114" s="6"/>
+      <c r="AC114" s="6"/>
+      <c r="AD114" s="6"/>
+    </row>
+    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -4524,8 +5266,13 @@
       <c r="W115" s="1"/>
       <c r="X115" s="1"/>
       <c r="Y115" s="1"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z115" s="1"/>
+      <c r="AA115" s="6"/>
+      <c r="AB115" s="6"/>
+      <c r="AC115" s="6"/>
+      <c r="AD115" s="6"/>
+    </row>
+    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -4551,8 +5298,13 @@
       <c r="W116" s="1"/>
       <c r="X116" s="1"/>
       <c r="Y116" s="1"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z116" s="1"/>
+      <c r="AA116" s="6"/>
+      <c r="AB116" s="6"/>
+      <c r="AC116" s="6"/>
+      <c r="AD116" s="6"/>
+    </row>
+    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -4578,8 +5330,13 @@
       <c r="W117" s="1"/>
       <c r="X117" s="1"/>
       <c r="Y117" s="1"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z117" s="1"/>
+      <c r="AA117" s="6"/>
+      <c r="AB117" s="6"/>
+      <c r="AC117" s="6"/>
+      <c r="AD117" s="6"/>
+    </row>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -4605,8 +5362,13 @@
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
       <c r="Y118" s="1"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z118" s="1"/>
+      <c r="AA118" s="6"/>
+      <c r="AB118" s="6"/>
+      <c r="AC118" s="6"/>
+      <c r="AD118" s="6"/>
+    </row>
+    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -4632,8 +5394,13 @@
       <c r="W119" s="1"/>
       <c r="X119" s="1"/>
       <c r="Y119" s="1"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z119" s="1"/>
+      <c r="AA119" s="6"/>
+      <c r="AB119" s="6"/>
+      <c r="AC119" s="6"/>
+      <c r="AD119" s="6"/>
+    </row>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -4659,8 +5426,13 @@
       <c r="W120" s="1"/>
       <c r="X120" s="1"/>
       <c r="Y120" s="1"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z120" s="1"/>
+      <c r="AA120" s="6"/>
+      <c r="AB120" s="6"/>
+      <c r="AC120" s="6"/>
+      <c r="AD120" s="6"/>
+    </row>
+    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -4686,8 +5458,13 @@
       <c r="W121" s="1"/>
       <c r="X121" s="1"/>
       <c r="Y121" s="1"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z121" s="1"/>
+      <c r="AA121" s="6"/>
+      <c r="AB121" s="6"/>
+      <c r="AC121" s="6"/>
+      <c r="AD121" s="6"/>
+    </row>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -4713,8 +5490,13 @@
       <c r="W122" s="1"/>
       <c r="X122" s="1"/>
       <c r="Y122" s="1"/>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z122" s="1"/>
+      <c r="AA122" s="6"/>
+      <c r="AB122" s="6"/>
+      <c r="AC122" s="6"/>
+      <c r="AD122" s="6"/>
+    </row>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -4740,8 +5522,13 @@
       <c r="W123" s="1"/>
       <c r="X123" s="1"/>
       <c r="Y123" s="1"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z123" s="1"/>
+      <c r="AA123" s="6"/>
+      <c r="AB123" s="6"/>
+      <c r="AC123" s="6"/>
+      <c r="AD123" s="6"/>
+    </row>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -4767,8 +5554,13 @@
       <c r="W124" s="1"/>
       <c r="X124" s="1"/>
       <c r="Y124" s="1"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z124" s="1"/>
+      <c r="AA124" s="6"/>
+      <c r="AB124" s="6"/>
+      <c r="AC124" s="6"/>
+      <c r="AD124" s="6"/>
+    </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -4794,8 +5586,13 @@
       <c r="W125" s="1"/>
       <c r="X125" s="1"/>
       <c r="Y125" s="1"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z125" s="1"/>
+      <c r="AA125" s="6"/>
+      <c r="AB125" s="6"/>
+      <c r="AC125" s="6"/>
+      <c r="AD125" s="6"/>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4821,8 +5618,13 @@
       <c r="W126" s="1"/>
       <c r="X126" s="1"/>
       <c r="Y126" s="1"/>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z126" s="1"/>
+      <c r="AA126" s="6"/>
+      <c r="AB126" s="6"/>
+      <c r="AC126" s="6"/>
+      <c r="AD126" s="6"/>
+    </row>
+    <row r="127" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -4848,8 +5650,13 @@
       <c r="W127" s="1"/>
       <c r="X127" s="1"/>
       <c r="Y127" s="1"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z127" s="1"/>
+      <c r="AA127" s="6"/>
+      <c r="AB127" s="6"/>
+      <c r="AC127" s="6"/>
+      <c r="AD127" s="6"/>
+    </row>
+    <row r="128" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -4875,8 +5682,13 @@
       <c r="W128" s="1"/>
       <c r="X128" s="1"/>
       <c r="Y128" s="1"/>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z128" s="1"/>
+      <c r="AA128" s="6"/>
+      <c r="AB128" s="6"/>
+      <c r="AC128" s="6"/>
+      <c r="AD128" s="6"/>
+    </row>
+    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -4902,8 +5714,13 @@
       <c r="W129" s="1"/>
       <c r="X129" s="1"/>
       <c r="Y129" s="1"/>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z129" s="1"/>
+      <c r="AA129" s="6"/>
+      <c r="AB129" s="6"/>
+      <c r="AC129" s="6"/>
+      <c r="AD129" s="6"/>
+    </row>
+    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -4929,8 +5746,13 @@
       <c r="W130" s="1"/>
       <c r="X130" s="1"/>
       <c r="Y130" s="1"/>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z130" s="1"/>
+      <c r="AA130" s="6"/>
+      <c r="AB130" s="6"/>
+      <c r="AC130" s="6"/>
+      <c r="AD130" s="6"/>
+    </row>
+    <row r="131" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -4956,8 +5778,13 @@
       <c r="W131" s="1"/>
       <c r="X131" s="1"/>
       <c r="Y131" s="1"/>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z131" s="1"/>
+      <c r="AA131" s="6"/>
+      <c r="AB131" s="6"/>
+      <c r="AC131" s="6"/>
+      <c r="AD131" s="6"/>
+    </row>
+    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -4983,8 +5810,13 @@
       <c r="W132" s="1"/>
       <c r="X132" s="1"/>
       <c r="Y132" s="1"/>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z132" s="1"/>
+      <c r="AA132" s="6"/>
+      <c r="AB132" s="6"/>
+      <c r="AC132" s="6"/>
+      <c r="AD132" s="6"/>
+    </row>
+    <row r="133" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -5010,8 +5842,13 @@
       <c r="W133" s="1"/>
       <c r="X133" s="1"/>
       <c r="Y133" s="1"/>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z133" s="1"/>
+      <c r="AA133" s="6"/>
+      <c r="AB133" s="6"/>
+      <c r="AC133" s="6"/>
+      <c r="AD133" s="6"/>
+    </row>
+    <row r="134" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -5037,8 +5874,13 @@
       <c r="W134" s="1"/>
       <c r="X134" s="1"/>
       <c r="Y134" s="1"/>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z134" s="1"/>
+      <c r="AA134" s="6"/>
+      <c r="AB134" s="6"/>
+      <c r="AC134" s="6"/>
+      <c r="AD134" s="6"/>
+    </row>
+    <row r="135" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -5064,8 +5906,13 @@
       <c r="W135" s="1"/>
       <c r="X135" s="1"/>
       <c r="Y135" s="1"/>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z135" s="1"/>
+      <c r="AA135" s="6"/>
+      <c r="AB135" s="6"/>
+      <c r="AC135" s="6"/>
+      <c r="AD135" s="6"/>
+    </row>
+    <row r="136" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -5091,8 +5938,13 @@
       <c r="W136" s="1"/>
       <c r="X136" s="1"/>
       <c r="Y136" s="1"/>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z136" s="1"/>
+      <c r="AA136" s="6"/>
+      <c r="AB136" s="6"/>
+      <c r="AC136" s="6"/>
+      <c r="AD136" s="6"/>
+    </row>
+    <row r="137" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -5118,8 +5970,13 @@
       <c r="W137" s="1"/>
       <c r="X137" s="1"/>
       <c r="Y137" s="1"/>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z137" s="1"/>
+      <c r="AA137" s="6"/>
+      <c r="AB137" s="6"/>
+      <c r="AC137" s="6"/>
+      <c r="AD137" s="6"/>
+    </row>
+    <row r="138" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -5145,8 +6002,13 @@
       <c r="W138" s="1"/>
       <c r="X138" s="1"/>
       <c r="Y138" s="1"/>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z138" s="1"/>
+      <c r="AA138" s="6"/>
+      <c r="AB138" s="6"/>
+      <c r="AC138" s="6"/>
+      <c r="AD138" s="6"/>
+    </row>
+    <row r="139" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -5172,8 +6034,13 @@
       <c r="W139" s="1"/>
       <c r="X139" s="1"/>
       <c r="Y139" s="1"/>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z139" s="1"/>
+      <c r="AA139" s="6"/>
+      <c r="AB139" s="6"/>
+      <c r="AC139" s="6"/>
+      <c r="AD139" s="6"/>
+    </row>
+    <row r="140" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -5199,8 +6066,13 @@
       <c r="W140" s="1"/>
       <c r="X140" s="1"/>
       <c r="Y140" s="1"/>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z140" s="1"/>
+      <c r="AA140" s="6"/>
+      <c r="AB140" s="6"/>
+      <c r="AC140" s="6"/>
+      <c r="AD140" s="6"/>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -5226,8 +6098,13 @@
       <c r="W141" s="1"/>
       <c r="X141" s="1"/>
       <c r="Y141" s="1"/>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z141" s="1"/>
+      <c r="AA141" s="6"/>
+      <c r="AB141" s="6"/>
+      <c r="AC141" s="6"/>
+      <c r="AD141" s="6"/>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -5253,8 +6130,13 @@
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
       <c r="Y142" s="1"/>
-    </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z142" s="1"/>
+      <c r="AA142" s="6"/>
+      <c r="AB142" s="6"/>
+      <c r="AC142" s="6"/>
+      <c r="AD142" s="6"/>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -5280,8 +6162,13 @@
       <c r="W143" s="1"/>
       <c r="X143" s="1"/>
       <c r="Y143" s="1"/>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z143" s="1"/>
+      <c r="AA143" s="6"/>
+      <c r="AB143" s="6"/>
+      <c r="AC143" s="6"/>
+      <c r="AD143" s="6"/>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -5307,8 +6194,13 @@
       <c r="W144" s="1"/>
       <c r="X144" s="1"/>
       <c r="Y144" s="1"/>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z144" s="1"/>
+      <c r="AA144" s="6"/>
+      <c r="AB144" s="6"/>
+      <c r="AC144" s="6"/>
+      <c r="AD144" s="6"/>
+    </row>
+    <row r="145" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -5334,8 +6226,13 @@
       <c r="W145" s="1"/>
       <c r="X145" s="1"/>
       <c r="Y145" s="1"/>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z145" s="1"/>
+      <c r="AA145" s="6"/>
+      <c r="AB145" s="6"/>
+      <c r="AC145" s="6"/>
+      <c r="AD145" s="6"/>
+    </row>
+    <row r="146" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -5361,8 +6258,13 @@
       <c r="W146" s="1"/>
       <c r="X146" s="1"/>
       <c r="Y146" s="1"/>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z146" s="1"/>
+      <c r="AA146" s="6"/>
+      <c r="AB146" s="6"/>
+      <c r="AC146" s="6"/>
+      <c r="AD146" s="6"/>
+    </row>
+    <row r="147" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -5388,8 +6290,13 @@
       <c r="W147" s="1"/>
       <c r="X147" s="1"/>
       <c r="Y147" s="1"/>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z147" s="1"/>
+      <c r="AA147" s="6"/>
+      <c r="AB147" s="6"/>
+      <c r="AC147" s="6"/>
+      <c r="AD147" s="6"/>
+    </row>
+    <row r="148" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -5415,8 +6322,13 @@
       <c r="W148" s="1"/>
       <c r="X148" s="1"/>
       <c r="Y148" s="1"/>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z148" s="1"/>
+      <c r="AA148" s="6"/>
+      <c r="AB148" s="6"/>
+      <c r="AC148" s="6"/>
+      <c r="AD148" s="6"/>
+    </row>
+    <row r="149" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -5442,8 +6354,13 @@
       <c r="W149" s="1"/>
       <c r="X149" s="1"/>
       <c r="Y149" s="1"/>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z149" s="1"/>
+      <c r="AA149" s="6"/>
+      <c r="AB149" s="6"/>
+      <c r="AC149" s="6"/>
+      <c r="AD149" s="6"/>
+    </row>
+    <row r="150" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -5469,8 +6386,13 @@
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
       <c r="Y150" s="1"/>
-    </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z150" s="1"/>
+      <c r="AA150" s="6"/>
+      <c r="AB150" s="6"/>
+      <c r="AC150" s="6"/>
+      <c r="AD150" s="6"/>
+    </row>
+    <row r="151" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -5496,8 +6418,13 @@
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
       <c r="Y151" s="1"/>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z151" s="1"/>
+      <c r="AA151" s="6"/>
+      <c r="AB151" s="6"/>
+      <c r="AC151" s="6"/>
+      <c r="AD151" s="6"/>
+    </row>
+    <row r="152" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -5523,8 +6450,13 @@
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
       <c r="Y152" s="1"/>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z152" s="1"/>
+      <c r="AA152" s="6"/>
+      <c r="AB152" s="6"/>
+      <c r="AC152" s="6"/>
+      <c r="AD152" s="6"/>
+    </row>
+    <row r="153" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -5550,8 +6482,13 @@
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
       <c r="Y153" s="1"/>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z153" s="1"/>
+      <c r="AA153" s="6"/>
+      <c r="AB153" s="6"/>
+      <c r="AC153" s="6"/>
+      <c r="AD153" s="6"/>
+    </row>
+    <row r="154" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -5577,8 +6514,13 @@
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
       <c r="Y154" s="1"/>
-    </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z154" s="1"/>
+      <c r="AA154" s="6"/>
+      <c r="AB154" s="6"/>
+      <c r="AC154" s="6"/>
+      <c r="AD154" s="6"/>
+    </row>
+    <row r="155" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -5604,8 +6546,13 @@
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
       <c r="Y155" s="1"/>
-    </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z155" s="1"/>
+      <c r="AA155" s="6"/>
+      <c r="AB155" s="6"/>
+      <c r="AC155" s="6"/>
+      <c r="AD155" s="6"/>
+    </row>
+    <row r="156" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -5631,8 +6578,13 @@
       <c r="W156" s="1"/>
       <c r="X156" s="1"/>
       <c r="Y156" s="1"/>
-    </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z156" s="1"/>
+      <c r="AA156" s="6"/>
+      <c r="AB156" s="6"/>
+      <c r="AC156" s="6"/>
+      <c r="AD156" s="6"/>
+    </row>
+    <row r="157" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -5658,8 +6610,13 @@
       <c r="W157" s="1"/>
       <c r="X157" s="1"/>
       <c r="Y157" s="1"/>
-    </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z157" s="1"/>
+      <c r="AA157" s="6"/>
+      <c r="AB157" s="6"/>
+      <c r="AC157" s="6"/>
+      <c r="AD157" s="6"/>
+    </row>
+    <row r="158" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -5685,8 +6642,13 @@
       <c r="W158" s="1"/>
       <c r="X158" s="1"/>
       <c r="Y158" s="1"/>
-    </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z158" s="1"/>
+      <c r="AA158" s="6"/>
+      <c r="AB158" s="6"/>
+      <c r="AC158" s="6"/>
+      <c r="AD158" s="6"/>
+    </row>
+    <row r="159" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -5712,8 +6674,13 @@
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
       <c r="Y159" s="1"/>
-    </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z159" s="1"/>
+      <c r="AA159" s="6"/>
+      <c r="AB159" s="6"/>
+      <c r="AC159" s="6"/>
+      <c r="AD159" s="6"/>
+    </row>
+    <row r="160" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -5739,8 +6706,13 @@
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
       <c r="Y160" s="1"/>
-    </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z160" s="1"/>
+      <c r="AA160" s="6"/>
+      <c r="AB160" s="6"/>
+      <c r="AC160" s="6"/>
+      <c r="AD160" s="6"/>
+    </row>
+    <row r="161" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5766,8 +6738,13 @@
       <c r="W161" s="1"/>
       <c r="X161" s="1"/>
       <c r="Y161" s="1"/>
-    </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z161" s="1"/>
+      <c r="AA161" s="6"/>
+      <c r="AB161" s="6"/>
+      <c r="AC161" s="6"/>
+      <c r="AD161" s="6"/>
+    </row>
+    <row r="162" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -5793,8 +6770,13 @@
       <c r="W162" s="1"/>
       <c r="X162" s="1"/>
       <c r="Y162" s="1"/>
-    </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z162" s="1"/>
+      <c r="AA162" s="6"/>
+      <c r="AB162" s="6"/>
+      <c r="AC162" s="6"/>
+      <c r="AD162" s="6"/>
+    </row>
+    <row r="163" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5820,8 +6802,13 @@
       <c r="W163" s="1"/>
       <c r="X163" s="1"/>
       <c r="Y163" s="1"/>
-    </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z163" s="1"/>
+      <c r="AA163" s="6"/>
+      <c r="AB163" s="6"/>
+      <c r="AC163" s="6"/>
+      <c r="AD163" s="6"/>
+    </row>
+    <row r="164" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5847,8 +6834,13 @@
       <c r="W164" s="1"/>
       <c r="X164" s="1"/>
       <c r="Y164" s="1"/>
-    </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z164" s="1"/>
+      <c r="AA164" s="6"/>
+      <c r="AB164" s="6"/>
+      <c r="AC164" s="6"/>
+      <c r="AD164" s="6"/>
+    </row>
+    <row r="165" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5874,8 +6866,13 @@
       <c r="W165" s="1"/>
       <c r="X165" s="1"/>
       <c r="Y165" s="1"/>
-    </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z165" s="1"/>
+      <c r="AA165" s="6"/>
+      <c r="AB165" s="6"/>
+      <c r="AC165" s="6"/>
+      <c r="AD165" s="6"/>
+    </row>
+    <row r="166" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5901,8 +6898,13 @@
       <c r="W166" s="1"/>
       <c r="X166" s="1"/>
       <c r="Y166" s="1"/>
-    </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z166" s="1"/>
+      <c r="AA166" s="6"/>
+      <c r="AB166" s="6"/>
+      <c r="AC166" s="6"/>
+      <c r="AD166" s="6"/>
+    </row>
+    <row r="167" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -5928,8 +6930,13 @@
       <c r="W167" s="1"/>
       <c r="X167" s="1"/>
       <c r="Y167" s="1"/>
-    </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z167" s="1"/>
+      <c r="AA167" s="6"/>
+      <c r="AB167" s="6"/>
+      <c r="AC167" s="6"/>
+      <c r="AD167" s="6"/>
+    </row>
+    <row r="168" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -5955,8 +6962,13 @@
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
       <c r="Y168" s="1"/>
-    </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z168" s="1"/>
+      <c r="AA168" s="6"/>
+      <c r="AB168" s="6"/>
+      <c r="AC168" s="6"/>
+      <c r="AD168" s="6"/>
+    </row>
+    <row r="169" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -5982,8 +6994,13 @@
       <c r="W169" s="1"/>
       <c r="X169" s="1"/>
       <c r="Y169" s="1"/>
-    </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z169" s="1"/>
+      <c r="AA169" s="6"/>
+      <c r="AB169" s="6"/>
+      <c r="AC169" s="6"/>
+      <c r="AD169" s="6"/>
+    </row>
+    <row r="170" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -6009,8 +7026,13 @@
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
       <c r="Y170" s="1"/>
-    </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z170" s="1"/>
+      <c r="AA170" s="6"/>
+      <c r="AB170" s="6"/>
+      <c r="AC170" s="6"/>
+      <c r="AD170" s="6"/>
+    </row>
+    <row r="171" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -6036,8 +7058,13 @@
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
       <c r="Y171" s="1"/>
-    </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z171" s="1"/>
+      <c r="AA171" s="6"/>
+      <c r="AB171" s="6"/>
+      <c r="AC171" s="6"/>
+      <c r="AD171" s="6"/>
+    </row>
+    <row r="172" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -6063,8 +7090,13 @@
       <c r="W172" s="1"/>
       <c r="X172" s="1"/>
       <c r="Y172" s="1"/>
-    </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z172" s="1"/>
+      <c r="AA172" s="6"/>
+      <c r="AB172" s="6"/>
+      <c r="AC172" s="6"/>
+      <c r="AD172" s="6"/>
+    </row>
+    <row r="173" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -6090,8 +7122,13 @@
       <c r="W173" s="1"/>
       <c r="X173" s="1"/>
       <c r="Y173" s="1"/>
-    </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z173" s="1"/>
+      <c r="AA173" s="6"/>
+      <c r="AB173" s="6"/>
+      <c r="AC173" s="6"/>
+      <c r="AD173" s="6"/>
+    </row>
+    <row r="174" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -6117,8 +7154,13 @@
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
       <c r="Y174" s="1"/>
-    </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z174" s="1"/>
+      <c r="AA174" s="6"/>
+      <c r="AB174" s="6"/>
+      <c r="AC174" s="6"/>
+      <c r="AD174" s="6"/>
+    </row>
+    <row r="175" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -6144,8 +7186,13 @@
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
       <c r="Y175" s="1"/>
-    </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z175" s="1"/>
+      <c r="AA175" s="6"/>
+      <c r="AB175" s="6"/>
+      <c r="AC175" s="6"/>
+      <c r="AD175" s="6"/>
+    </row>
+    <row r="176" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -6171,8 +7218,13 @@
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
       <c r="Y176" s="1"/>
-    </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z176" s="1"/>
+      <c r="AA176" s="6"/>
+      <c r="AB176" s="6"/>
+      <c r="AC176" s="6"/>
+      <c r="AD176" s="6"/>
+    </row>
+    <row r="177" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -6198,8 +7250,13 @@
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
       <c r="Y177" s="1"/>
-    </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z177" s="1"/>
+      <c r="AA177" s="6"/>
+      <c r="AB177" s="6"/>
+      <c r="AC177" s="6"/>
+      <c r="AD177" s="6"/>
+    </row>
+    <row r="178" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -6225,8 +7282,13 @@
       <c r="W178" s="1"/>
       <c r="X178" s="1"/>
       <c r="Y178" s="1"/>
-    </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z178" s="1"/>
+      <c r="AA178" s="6"/>
+      <c r="AB178" s="6"/>
+      <c r="AC178" s="6"/>
+      <c r="AD178" s="6"/>
+    </row>
+    <row r="179" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -6252,8 +7314,13 @@
       <c r="W179" s="1"/>
       <c r="X179" s="1"/>
       <c r="Y179" s="1"/>
-    </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z179" s="1"/>
+      <c r="AA179" s="6"/>
+      <c r="AB179" s="6"/>
+      <c r="AC179" s="6"/>
+      <c r="AD179" s="6"/>
+    </row>
+    <row r="180" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -6279,8 +7346,13 @@
       <c r="W180" s="1"/>
       <c r="X180" s="1"/>
       <c r="Y180" s="1"/>
-    </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z180" s="1"/>
+      <c r="AA180" s="6"/>
+      <c r="AB180" s="6"/>
+      <c r="AC180" s="6"/>
+      <c r="AD180" s="6"/>
+    </row>
+    <row r="181" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -6306,8 +7378,13 @@
       <c r="W181" s="1"/>
       <c r="X181" s="1"/>
       <c r="Y181" s="1"/>
-    </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z181" s="1"/>
+      <c r="AA181" s="6"/>
+      <c r="AB181" s="6"/>
+      <c r="AC181" s="6"/>
+      <c r="AD181" s="6"/>
+    </row>
+    <row r="182" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -6333,8 +7410,13 @@
       <c r="W182" s="1"/>
       <c r="X182" s="1"/>
       <c r="Y182" s="1"/>
-    </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z182" s="1"/>
+      <c r="AA182" s="6"/>
+      <c r="AB182" s="6"/>
+      <c r="AC182" s="6"/>
+      <c r="AD182" s="6"/>
+    </row>
+    <row r="183" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -6360,8 +7442,13 @@
       <c r="W183" s="1"/>
       <c r="X183" s="1"/>
       <c r="Y183" s="1"/>
-    </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z183" s="1"/>
+      <c r="AA183" s="6"/>
+      <c r="AB183" s="6"/>
+      <c r="AC183" s="6"/>
+      <c r="AD183" s="6"/>
+    </row>
+    <row r="184" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -6387,8 +7474,13 @@
       <c r="W184" s="1"/>
       <c r="X184" s="1"/>
       <c r="Y184" s="1"/>
-    </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z184" s="1"/>
+      <c r="AA184" s="6"/>
+      <c r="AB184" s="6"/>
+      <c r="AC184" s="6"/>
+      <c r="AD184" s="6"/>
+    </row>
+    <row r="185" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -6414,8 +7506,13 @@
       <c r="W185" s="1"/>
       <c r="X185" s="1"/>
       <c r="Y185" s="1"/>
-    </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z185" s="1"/>
+      <c r="AA185" s="6"/>
+      <c r="AB185" s="6"/>
+      <c r="AC185" s="6"/>
+      <c r="AD185" s="6"/>
+    </row>
+    <row r="186" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -6441,8 +7538,13 @@
       <c r="W186" s="1"/>
       <c r="X186" s="1"/>
       <c r="Y186" s="1"/>
-    </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z186" s="1"/>
+      <c r="AA186" s="6"/>
+      <c r="AB186" s="6"/>
+      <c r="AC186" s="6"/>
+      <c r="AD186" s="6"/>
+    </row>
+    <row r="187" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -6468,8 +7570,13 @@
       <c r="W187" s="1"/>
       <c r="X187" s="1"/>
       <c r="Y187" s="1"/>
-    </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z187" s="1"/>
+      <c r="AA187" s="6"/>
+      <c r="AB187" s="6"/>
+      <c r="AC187" s="6"/>
+      <c r="AD187" s="6"/>
+    </row>
+    <row r="188" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -6495,8 +7602,13 @@
       <c r="W188" s="1"/>
       <c r="X188" s="1"/>
       <c r="Y188" s="1"/>
-    </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z188" s="1"/>
+      <c r="AA188" s="6"/>
+      <c r="AB188" s="6"/>
+      <c r="AC188" s="6"/>
+      <c r="AD188" s="6"/>
+    </row>
+    <row r="189" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -6522,8 +7634,13 @@
       <c r="W189" s="1"/>
       <c r="X189" s="1"/>
       <c r="Y189" s="1"/>
-    </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z189" s="1"/>
+      <c r="AA189" s="6"/>
+      <c r="AB189" s="6"/>
+      <c r="AC189" s="6"/>
+      <c r="AD189" s="6"/>
+    </row>
+    <row r="190" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -6549,8 +7666,13 @@
       <c r="W190" s="1"/>
       <c r="X190" s="1"/>
       <c r="Y190" s="1"/>
-    </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z190" s="1"/>
+      <c r="AA190" s="6"/>
+      <c r="AB190" s="6"/>
+      <c r="AC190" s="6"/>
+      <c r="AD190" s="6"/>
+    </row>
+    <row r="191" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -6576,8 +7698,13 @@
       <c r="W191" s="1"/>
       <c r="X191" s="1"/>
       <c r="Y191" s="1"/>
-    </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z191" s="1"/>
+      <c r="AA191" s="6"/>
+      <c r="AB191" s="6"/>
+      <c r="AC191" s="6"/>
+      <c r="AD191" s="6"/>
+    </row>
+    <row r="192" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -6603,8 +7730,13 @@
       <c r="W192" s="1"/>
       <c r="X192" s="1"/>
       <c r="Y192" s="1"/>
-    </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z192" s="1"/>
+      <c r="AA192" s="6"/>
+      <c r="AB192" s="6"/>
+      <c r="AC192" s="6"/>
+      <c r="AD192" s="6"/>
+    </row>
+    <row r="193" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -6630,8 +7762,13 @@
       <c r="W193" s="1"/>
       <c r="X193" s="1"/>
       <c r="Y193" s="1"/>
-    </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z193" s="1"/>
+      <c r="AA193" s="6"/>
+      <c r="AB193" s="6"/>
+      <c r="AC193" s="6"/>
+      <c r="AD193" s="6"/>
+    </row>
+    <row r="194" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -6657,8 +7794,13 @@
       <c r="W194" s="1"/>
       <c r="X194" s="1"/>
       <c r="Y194" s="1"/>
-    </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z194" s="1"/>
+      <c r="AA194" s="6"/>
+      <c r="AB194" s="6"/>
+      <c r="AC194" s="6"/>
+      <c r="AD194" s="6"/>
+    </row>
+    <row r="195" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -6684,8 +7826,13 @@
       <c r="W195" s="1"/>
       <c r="X195" s="1"/>
       <c r="Y195" s="1"/>
-    </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z195" s="1"/>
+      <c r="AA195" s="6"/>
+      <c r="AB195" s="6"/>
+      <c r="AC195" s="6"/>
+      <c r="AD195" s="6"/>
+    </row>
+    <row r="196" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -6711,8 +7858,13 @@
       <c r="W196" s="1"/>
       <c r="X196" s="1"/>
       <c r="Y196" s="1"/>
-    </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z196" s="1"/>
+      <c r="AA196" s="6"/>
+      <c r="AB196" s="6"/>
+      <c r="AC196" s="6"/>
+      <c r="AD196" s="6"/>
+    </row>
+    <row r="197" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -6738,8 +7890,13 @@
       <c r="W197" s="1"/>
       <c r="X197" s="1"/>
       <c r="Y197" s="1"/>
-    </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z197" s="1"/>
+      <c r="AA197" s="6"/>
+      <c r="AB197" s="6"/>
+      <c r="AC197" s="6"/>
+      <c r="AD197" s="6"/>
+    </row>
+    <row r="198" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -6765,8 +7922,13 @@
       <c r="W198" s="1"/>
       <c r="X198" s="1"/>
       <c r="Y198" s="1"/>
-    </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z198" s="1"/>
+      <c r="AA198" s="6"/>
+      <c r="AB198" s="6"/>
+      <c r="AC198" s="6"/>
+      <c r="AD198" s="6"/>
+    </row>
+    <row r="199" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -6792,8 +7954,13 @@
       <c r="W199" s="1"/>
       <c r="X199" s="1"/>
       <c r="Y199" s="1"/>
-    </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z199" s="1"/>
+      <c r="AA199" s="6"/>
+      <c r="AB199" s="6"/>
+      <c r="AC199" s="6"/>
+      <c r="AD199" s="6"/>
+    </row>
+    <row r="200" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -6819,15 +7986,21 @@
       <c r="W200" s="1"/>
       <c r="X200" s="1"/>
       <c r="Y200" s="1"/>
+      <c r="Z200" s="1"/>
+      <c r="AA200" s="6"/>
+      <c r="AB200" s="6"/>
+      <c r="AC200" s="6"/>
+      <c r="AD200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="T1:Y1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="L1:S1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="T1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjustment on in the allowance and unworked hours.
</commit_message>
<xml_diff>
--- a/storage/system/master.xlsx
+++ b/storage/system/master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\payhp\storage\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9435E8-1EA1-4BC8-8A7C-5405401662CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2960DC2-0DE7-4DCC-B982-A0ECE5D0F261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,7 +1756,7 @@
         <v>500</v>
       </c>
       <c r="K7" s="1">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="L7" s="1">
         <v>500</v>

</xml_diff>